<commit_message>
Updated 24V test data
</commit_message>
<xml_diff>
--- a/Test Data/Verify_24V_Load_On_Addition_Deletion_Of_Accessories.xlsx
+++ b/Test Data/Verify_24V_Load_On_Addition_Deletion_Of_Accessories.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792D6F2F-EFA4-4787-B21D-D17D9B223C94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels and Devices" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -123,7 +122,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -526,11 +525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,7 +650,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="2">
-        <v>0.39300000000000002</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>24</v>
@@ -663,10 +662,10 @@
         <v>26</v>
       </c>
       <c r="J8" s="2">
-        <v>0.44500000000000001</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="K8" s="2">
-        <v>0.39300000000000002</v>
+        <v>0.32900000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 24V test cases and test data with new loading details method
</commit_message>
<xml_diff>
--- a/Test Data/Verify_24V_Load_On_Addition_Deletion_Of_Accessories.xlsx
+++ b/Test Data/Verify_24V_Load_On_Addition_Deletion_Of_Accessories.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\consys-uiauto\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61E7864-F2F2-4190-A000-6C5289B91EFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels and Devices" sheetId="6" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Color Codes</t>
   </si>
@@ -117,12 +112,18 @@
   </si>
   <si>
     <t>Verify 24V PSU Load on addition and deletion of Accessories</t>
+  </si>
+  <si>
+    <t>Loading Details Name</t>
+  </si>
+  <si>
+    <t>Main Processor 24V (A)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -219,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -245,6 +246,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,11 +529,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,9 +547,10 @@
     <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="19.5546875" customWidth="1"/>
     <col min="10" max="11" width="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -553,7 +558,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -565,7 +570,7 @@
       </c>
       <c r="D2" s="13"/>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -577,7 +582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -589,16 +594,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
     </row>
-    <row r="7" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -632,8 +637,11 @@
       <c r="K7" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -666,6 +674,9 @@
       </c>
       <c r="K8" s="2">
         <v>0.32900000000000001</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>